<commit_message>
WIP - Create mappings template
</commit_message>
<xml_diff>
--- a/data/input/dagstuhl2024/Example - GDP and Employment.xlsx
+++ b/data/input/dagstuhl2024/Example - GDP and Employment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\CDIF\undata_example_cdif\data\input\dagstuhl2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51D44F6-CD8F-4DC2-AF0A-13745819E169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBAFCDB-4066-404A-9F03-48735949FFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{70BD51A8-8392-48D0-AC17-D5B5047A2F43}"/>
   </bookViews>
@@ -2847,7 +2847,7 @@
   <dimension ref="A1:F169"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
code and data cleanup
</commit_message>
<xml_diff>
--- a/data/input/dagstuhl2024/Example - GDP and Employment.xlsx
+++ b/data/input/dagstuhl2024/Example - GDP and Employment.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\CDIF\undata_example_cdif\data\input\dagstuhl2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBAFCDB-4066-404A-9F03-48735949FFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E21969-2D30-41BB-B773-874DB49B6760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{70BD51A8-8392-48D0-AC17-D5B5047A2F43}"/>
+    <workbookView xWindow="1776" yWindow="1776" windowWidth="17280" windowHeight="8880" xr2:uid="{70BD51A8-8392-48D0-AC17-D5B5047A2F43}"/>
   </bookViews>
   <sheets>
     <sheet name="GDP_DATA" sheetId="1" r:id="rId1"/>
     <sheet name="CL_REF_AREA" sheetId="2" r:id="rId2"/>
     <sheet name="CL_EC2" sheetId="3" r:id="rId3"/>
-    <sheet name="EMPLOYMENT_DATA" sheetId="5" r:id="rId4"/>
+    <sheet name="UNEMPLOYMENT_DATA" sheetId="5" r:id="rId4"/>
     <sheet name="CL_SEX" sheetId="8" r:id="rId5"/>
     <sheet name="CL_ACTIVITY" sheetId="7" r:id="rId6"/>
     <sheet name="CL_COUNTRY" sheetId="6" r:id="rId7"/>
@@ -230,7 +230,7 @@
     <t>USD</t>
   </si>
   <si>
-    <t>EMPLOYMENT_RATE (Percent)</t>
+    <t>UNEMPLOYMENT_RATE (Percent)</t>
   </si>
 </sst>
 </file>
@@ -720,9 +720,7 @@
   </sheetPr>
   <dimension ref="A1:G83"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2846,8 +2844,8 @@
   </sheetPr>
   <dimension ref="A1:F169"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Example up to mappings
</commit_message>
<xml_diff>
--- a/data/input/dagstuhl2024/Example - GDP and Employment.xlsx
+++ b/data/input/dagstuhl2024/Example - GDP and Employment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\CDIF\undata_example_cdif\data\input\dagstuhl2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E21969-2D30-41BB-B773-874DB49B6760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82C40AE-C1ED-4275-903F-5E359153DCEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1776" yWindow="1776" windowWidth="17280" windowHeight="8880" xr2:uid="{70BD51A8-8392-48D0-AC17-D5B5047A2F43}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{70BD51A8-8392-48D0-AC17-D5B5047A2F43}"/>
   </bookViews>
   <sheets>
     <sheet name="GDP_DATA" sheetId="1" r:id="rId1"/>
@@ -720,7 +720,7 @@
   </sheetPr>
   <dimension ref="A1:G83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2844,7 +2844,7 @@
   </sheetPr>
   <dimension ref="A1:F169"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>